<commit_message>
Got Least Squares Working. Updated Monte Carlo using Least Squares Solution
</commit_message>
<xml_diff>
--- a/TdoaSim/Table Pasting sheet for TDoA Algorithm.xlsx
+++ b/TdoaSim/Table Pasting sheet for TDoA Algorithm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awian\Desktop\MSD\FeasibilityStudies\TdoaSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD83DE7-6A65-4CAE-BC4F-5294F7EA6333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A966EC6E-C5AE-4EE9-88C7-3C0526A44447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9C80441F-F6AE-4DB9-852C-59754C43E2C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9C80441F-F6AE-4DB9-852C-59754C43E2C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>NaN</t>
   </si>
@@ -389,26 +389,26 @@
     <xf numFmtId="9" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -727,18 +727,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B51845-1427-495A-BD73-7D4E95FCEF8A}">
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="Q47" sqref="Q47:AA56"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:K53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>55.705077356707001</v>
       </c>
@@ -746,7 +746,7 @@
         <v>96.067873360791097</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>55.889128192706799</v>
       </c>
@@ -754,7 +754,7 @@
         <v>63.839557199669798</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3.2124944277779499</v>
       </c>
@@ -762,7 +762,7 @@
         <v>93.641939863245895</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44.164760288599602</v>
       </c>
@@ -773,7 +773,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>30.660925448314298</v>
       </c>
@@ -799,7 +799,7 @@
         <v>9.6313058976432195</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>64.457434689864698</v>
       </c>
@@ -825,7 +825,7 @@
         <v>1.86844549323231</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>31.7511468577332</v>
       </c>
@@ -851,7 +851,7 @@
         <v>0.47713111411165299</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>69.715922611137799</v>
       </c>
@@ -877,7 +877,7 @@
         <v>3.5599559739866501E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>61.222716668093497</v>
       </c>
@@ -903,7 +903,7 @@
         <v>9.1470221605850798E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>48.607534868386999</v>
       </c>
@@ -929,7 +929,7 @@
         <v>2.61817654237816E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="P12">
         <v>120</v>
       </c>
@@ -949,7 +949,7 @@
         <v>5.0068132382035998E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="P13">
         <v>120</v>
       </c>
@@ -969,7 +969,7 @@
         <v>2.4406635444539802E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>55.705077356707001</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>6.0859702966159497E-15</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>96.067873360791097</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>259.22135497745398</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="P16">
         <v>260</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>1969.7380324969699</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1112,24 +1112,24 @@
         <v>257.73860303978898</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>0.99691358024691401</v>
       </c>
       <c r="B18" s="3">
-        <v>0.65277777777777801</v>
+        <v>0.72376543209876498</v>
       </c>
       <c r="C18" s="23">
-        <v>4.47253967987099</v>
+        <v>4.7671038831319503</v>
       </c>
       <c r="D18" s="23">
-        <v>8.2914413734249095</v>
+        <v>7.3886384856665499</v>
       </c>
       <c r="E18" s="23">
-        <v>3.7221787163423001</v>
+        <v>3.9187364944388201</v>
       </c>
       <c r="F18" s="23">
-        <v>1.69699249272632</v>
+        <v>1.8312892685683</v>
       </c>
       <c r="G18" s="2">
         <v>5</v>
@@ -1138,102 +1138,102 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>0.99537037037037002</v>
       </c>
       <c r="B19" s="3">
-        <v>0.66975308641975295</v>
+        <v>0.78395061728395099</v>
       </c>
       <c r="C19" s="23">
-        <v>3.6377394245540402</v>
+        <v>3.7662814815966699</v>
       </c>
       <c r="D19" s="23">
-        <v>5.7765235180054102</v>
+        <v>4.8888570983064898</v>
       </c>
       <c r="E19" s="23">
-        <v>3.06166714185956</v>
+        <v>3.2957187729732502</v>
       </c>
       <c r="F19" s="23">
-        <v>1.2589285701489901</v>
+        <v>1.6489958987211799</v>
       </c>
       <c r="G19" s="2">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H19">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>0.842592592592593</v>
       </c>
       <c r="B20" s="3">
-        <v>0</v>
+        <v>6.17283950617284E-3</v>
       </c>
       <c r="C20" s="23">
-        <v>51.255428491375298</v>
+        <v>140.23229899214101</v>
       </c>
       <c r="D20" s="23">
-        <v>186.04237009164601</v>
+        <v>96.5967390467179</v>
       </c>
       <c r="E20" s="23">
-        <v>20.7243620934916</v>
+        <v>18.732482482163</v>
       </c>
       <c r="F20" s="23">
-        <v>15.8486714208561</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>0</v>
+        <v>11.8924443740201</v>
+      </c>
+      <c r="G20" s="2">
+        <v>90</v>
       </c>
       <c r="H20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>0.99691358024691401</v>
       </c>
       <c r="B21" s="3">
-        <v>0.594135802469136</v>
+        <v>0.69598765432098797</v>
       </c>
       <c r="C21" s="23">
-        <v>5.1820091781824296</v>
+        <v>5.6257518742842203</v>
       </c>
       <c r="D21" s="23">
-        <v>9.3529051297731804</v>
+        <v>7.7493487546476496</v>
       </c>
       <c r="E21" s="23">
-        <v>4.1489373827683202</v>
+        <v>4.2957494487215797</v>
       </c>
       <c r="F21" s="23">
-        <v>1.6579919279144</v>
+        <v>1.81313465856018</v>
       </c>
       <c r="G21" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H21">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>0.99228395061728403</v>
       </c>
       <c r="B22" s="3">
-        <v>0.50771604938271597</v>
+        <v>0.50925925925925897</v>
       </c>
       <c r="C22" s="23">
-        <v>8.6894047563383392</v>
+        <v>9.2382514597639496</v>
       </c>
       <c r="D22" s="23">
-        <v>15.308949731927401</v>
+        <v>16.767183749549101</v>
       </c>
       <c r="E22" s="23">
-        <v>6.2931434326642099</v>
+        <v>6.4116686665628002</v>
       </c>
       <c r="F22" s="23">
-        <v>2.19869393554493</v>
+        <v>2.1090802280016301</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>0</v>
@@ -1242,76 +1242,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>0.99691358024691401</v>
       </c>
       <c r="B23" s="3">
-        <v>0.72376543209876498</v>
+        <v>0.81481481481481499</v>
       </c>
       <c r="C23" s="23">
-        <v>3.15094556693525</v>
+        <v>3.5189800132604701</v>
       </c>
       <c r="D23" s="23">
-        <v>4.7272303779212503</v>
+        <v>3.8136691510956102</v>
       </c>
       <c r="E23" s="23">
-        <v>2.7564970850756301</v>
+        <v>2.8499983421883202</v>
       </c>
       <c r="F23" s="23">
-        <v>1.3300341564986999</v>
+        <v>1.5828147353200701</v>
       </c>
       <c r="G23" s="2">
         <v>5</v>
       </c>
       <c r="H23">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>0.99228395061728403</v>
       </c>
       <c r="B24" s="3">
-        <v>0.50617283950617298</v>
+        <v>0.56018518518518501</v>
       </c>
       <c r="C24" s="23">
-        <v>8.0320091327366203</v>
+        <v>8.5484976442793297</v>
       </c>
       <c r="D24" s="23">
-        <v>18.246567398679598</v>
+        <v>12.826225709224101</v>
       </c>
       <c r="E24" s="23">
-        <v>5.6719759878125204</v>
+        <v>5.8030763884773204</v>
       </c>
       <c r="F24" s="23">
-        <v>1.7528987497512301</v>
+        <v>1.7579508362319101</v>
       </c>
       <c r="G24" s="2">
         <v>30</v>
       </c>
       <c r="H24">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>0.99845679012345701</v>
       </c>
       <c r="B25" s="3">
-        <v>0.73919753086419804</v>
+        <v>0.82253086419753096</v>
       </c>
       <c r="C25" s="23">
-        <v>2.9980170630850802</v>
+        <v>3.2274161884264401</v>
       </c>
       <c r="D25" s="23">
-        <v>5.2186097613921998</v>
+        <v>3.8777858727358701</v>
       </c>
       <c r="E25" s="23">
-        <v>2.66436933930542</v>
+        <v>2.76065726625606</v>
       </c>
       <c r="F25" s="23">
-        <v>1.3188221759768499</v>
+        <v>1.6268928954965201</v>
       </c>
       <c r="G25" s="2">
         <v>5</v>
@@ -1320,24 +1320,24 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>0.99691358024691401</v>
       </c>
       <c r="B26" s="3">
-        <v>0.70524691358024705</v>
+        <v>0.80555555555555602</v>
       </c>
       <c r="C26" s="23">
-        <v>3.3362927130072499</v>
+        <v>3.6042473989701298</v>
       </c>
       <c r="D26" s="23">
-        <v>5.2201145779597198</v>
+        <v>4.2251748337440098</v>
       </c>
       <c r="E26" s="23">
-        <v>2.8513275994396499</v>
+        <v>3.0511811971656901</v>
       </c>
       <c r="F26" s="23">
-        <v>1.2982012651313799</v>
+        <v>1.55722525088334</v>
       </c>
       <c r="G26" s="2">
         <v>5</v>
@@ -1346,34 +1346,34 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>0.99537037037037002</v>
       </c>
       <c r="B27" s="3">
-        <v>0.66666666666666696</v>
+        <v>0.72530864197530898</v>
       </c>
       <c r="C27" s="23">
-        <v>4.7716764512370702</v>
+        <v>4.9603323128851198</v>
       </c>
       <c r="D27" s="23">
-        <v>7.3898864727209297</v>
+        <v>6.8773124311142899</v>
       </c>
       <c r="E27" s="23">
-        <v>3.7832890483244102</v>
+        <v>3.9077700402310001</v>
       </c>
       <c r="F27" s="23">
-        <v>1.55703743983555</v>
+        <v>1.65377294417689</v>
       </c>
       <c r="G27" s="2">
         <v>5</v>
       </c>
       <c r="H27">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:21" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:21" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="16" t="s">
         <v>5</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:21" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="17" t="s">
         <v>7</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="47.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:21" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>9</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="47.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:27" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="7" t="s">
         <v>6</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="70.8" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:27" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="7" t="s">
         <v>12</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="47.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:27" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="18" t="s">
         <v>3</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="47.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:27" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="13" t="s">
         <v>4</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="70.8" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:27" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="10" t="s">
         <v>11</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="70.8" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:27" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="10" t="s">
         <v>8</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="70.8" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:27" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
         <v>10</v>
       </c>
@@ -1693,59 +1693,59 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:27" ht="117" x14ac:dyDescent="0.3">
-      <c r="A42" s="34" t="s">
+    <row r="41" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:27" ht="116.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="34" t="s">
+      <c r="B42" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="39" t="s">
         <v>17</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="F42" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="34" t="s">
+      <c r="G42" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="I42" s="34" t="s">
+      <c r="I42" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="34" t="s">
+      <c r="J42" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="K42" s="34" t="s">
+      <c r="K42" s="39" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
+    <row r="43" spans="1:27" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
       <c r="E43" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
-    </row>
-    <row r="44" spans="1:27" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="36" t="s">
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="40"/>
+    </row>
+    <row r="44" spans="1:27" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="34" t="s">
         <v>5</v>
       </c>
       <c r="B44" s="26">
@@ -1757,29 +1757,29 @@
       <c r="D44" s="27">
         <v>0.84</v>
       </c>
-      <c r="E44" s="27">
-        <v>0</v>
-      </c>
-      <c r="F44" s="26">
-        <v>51.3</v>
-      </c>
-      <c r="G44" s="26">
-        <v>186</v>
-      </c>
-      <c r="H44" s="26">
-        <v>20.7</v>
-      </c>
-      <c r="I44" s="26">
-        <v>15.8</v>
-      </c>
-      <c r="J44" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="K44" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27" ht="47.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E44" s="3">
+        <v>6.17283950617284E-3</v>
+      </c>
+      <c r="F44" s="23">
+        <v>140.23229899214101</v>
+      </c>
+      <c r="G44" s="23">
+        <v>96.5967390467179</v>
+      </c>
+      <c r="H44" s="23">
+        <v>18.732482482163</v>
+      </c>
+      <c r="I44" s="23">
+        <v>11.8924443740201</v>
+      </c>
+      <c r="J44" s="2">
+        <v>90</v>
+      </c>
+      <c r="K44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="31" t="s">
         <v>7</v>
       </c>
@@ -1792,29 +1792,29 @@
       <c r="D45" s="33">
         <v>0.99</v>
       </c>
-      <c r="E45" s="33">
-        <v>0.51</v>
-      </c>
-      <c r="F45" s="32">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="G45" s="32">
-        <v>15.3</v>
-      </c>
-      <c r="H45" s="32">
-        <v>6.3</v>
-      </c>
-      <c r="I45" s="32">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J45" s="32" t="s">
+      <c r="E45" s="3">
+        <v>0.50925925925925897</v>
+      </c>
+      <c r="F45" s="23">
+        <v>9.2382514597639496</v>
+      </c>
+      <c r="G45" s="23">
+        <v>16.767183749549101</v>
+      </c>
+      <c r="H45" s="23">
+        <v>6.4116686665628002</v>
+      </c>
+      <c r="I45" s="23">
+        <v>2.1090802280016301</v>
+      </c>
+      <c r="J45" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K45" s="32">
+      <c r="K45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="47.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:27" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="31" t="s">
         <v>9</v>
       </c>
@@ -1827,29 +1827,29 @@
       <c r="D46" s="33">
         <v>0.99</v>
       </c>
-      <c r="E46" s="33">
-        <v>0.51</v>
-      </c>
-      <c r="F46" s="32">
-        <v>8</v>
-      </c>
-      <c r="G46" s="32">
-        <v>18.2</v>
-      </c>
-      <c r="H46" s="32">
-        <v>5.7</v>
-      </c>
-      <c r="I46" s="32">
-        <v>1.8</v>
-      </c>
-      <c r="J46" s="32">
+      <c r="E46" s="3">
+        <v>0.56018518518518501</v>
+      </c>
+      <c r="F46" s="23">
+        <v>8.5484976442793297</v>
+      </c>
+      <c r="G46" s="23">
+        <v>12.826225709224101</v>
+      </c>
+      <c r="H46" s="23">
+        <v>5.8030763884773204</v>
+      </c>
+      <c r="I46" s="23">
+        <v>1.7579508362319101</v>
+      </c>
+      <c r="J46" s="2">
         <v>30</v>
       </c>
-      <c r="K46" s="32">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27" ht="47.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="28" t="s">
         <v>6</v>
       </c>
@@ -1862,62 +1862,62 @@
       <c r="D47" s="30">
         <v>1</v>
       </c>
-      <c r="E47" s="30">
-        <v>0.59</v>
-      </c>
-      <c r="F47" s="29">
-        <v>5.2</v>
-      </c>
-      <c r="G47" s="29">
-        <v>9.4</v>
-      </c>
-      <c r="H47" s="29">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I47" s="29">
-        <v>1.7</v>
-      </c>
-      <c r="J47" s="29">
-        <v>10</v>
-      </c>
-      <c r="K47" s="29">
-        <v>55</v>
-      </c>
-      <c r="Q47" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="R47" s="39">
+      <c r="E47" s="3">
+        <v>0.69598765432098797</v>
+      </c>
+      <c r="F47" s="23">
+        <v>5.6257518742842203</v>
+      </c>
+      <c r="G47" s="23">
+        <v>7.7493487546476496</v>
+      </c>
+      <c r="H47" s="23">
+        <v>4.2957494487215797</v>
+      </c>
+      <c r="I47" s="23">
+        <v>1.81313465856018</v>
+      </c>
+      <c r="J47" s="2">
+        <v>15</v>
+      </c>
+      <c r="K47">
+        <v>50</v>
+      </c>
+      <c r="Q47" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="R47" s="37">
         <v>3</v>
       </c>
-      <c r="S47" s="39">
+      <c r="S47" s="37">
         <v>94</v>
       </c>
-      <c r="T47" s="40">
+      <c r="T47" s="38">
         <v>0.84</v>
       </c>
-      <c r="U47" s="40">
+      <c r="U47" s="38">
         <v>0</v>
       </c>
-      <c r="V47" s="39">
+      <c r="V47" s="37">
         <v>51.3</v>
       </c>
-      <c r="W47" s="39">
+      <c r="W47" s="37">
         <v>186</v>
       </c>
-      <c r="X47" s="39">
+      <c r="X47" s="37">
         <v>20.7</v>
       </c>
-      <c r="Y47" s="39">
+      <c r="Y47" s="37">
         <v>15.8</v>
       </c>
-      <c r="Z47" s="39" t="s">
+      <c r="Z47" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="AA47" s="39">
+      <c r="AA47" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="71.400000000000006" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:27" ht="71.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="28" t="s">
         <v>12</v>
       </c>
@@ -1930,28 +1930,28 @@
       <c r="D48" s="30">
         <v>1</v>
       </c>
-      <c r="E48" s="30">
-        <v>0.67</v>
-      </c>
-      <c r="F48" s="29">
-        <v>4.8</v>
-      </c>
-      <c r="G48" s="29">
-        <v>7.4</v>
-      </c>
-      <c r="H48" s="29">
-        <v>3.8</v>
-      </c>
-      <c r="I48" s="29">
-        <v>1.6</v>
-      </c>
-      <c r="J48" s="29">
-        <v>5</v>
-      </c>
-      <c r="K48" s="29">
-        <v>55</v>
-      </c>
-      <c r="Q48" s="36" t="s">
+      <c r="E48" s="3">
+        <v>0.72530864197530898</v>
+      </c>
+      <c r="F48" s="23">
+        <v>4.9603323128851198</v>
+      </c>
+      <c r="G48" s="23">
+        <v>6.8773124311142899</v>
+      </c>
+      <c r="H48" s="23">
+        <v>3.9077700402310001</v>
+      </c>
+      <c r="I48" s="23">
+        <v>1.65377294417689</v>
+      </c>
+      <c r="J48" s="2">
+        <v>5</v>
+      </c>
+      <c r="K48">
+        <v>60</v>
+      </c>
+      <c r="Q48" s="34" t="s">
         <v>7</v>
       </c>
       <c r="R48" s="26">
@@ -1985,8 +1985,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="93.6" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A49" s="37" t="s">
+    <row r="49" spans="1:27" ht="93.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="35" t="s">
         <v>26</v>
       </c>
       <c r="B49" s="32">
@@ -1998,25 +1998,25 @@
       <c r="D49" s="33">
         <v>1</v>
       </c>
-      <c r="E49" s="33">
-        <v>0.65</v>
-      </c>
-      <c r="F49" s="32">
-        <v>4.5</v>
-      </c>
-      <c r="G49" s="32">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="H49" s="32">
-        <v>3.7</v>
-      </c>
-      <c r="I49" s="32">
-        <v>1.7</v>
-      </c>
-      <c r="J49" s="32">
-        <v>5</v>
-      </c>
-      <c r="K49" s="32">
+      <c r="E49" s="3">
+        <v>0.72376543209876498</v>
+      </c>
+      <c r="F49" s="23">
+        <v>4.7671038831319503</v>
+      </c>
+      <c r="G49" s="23">
+        <v>7.3886384856665499</v>
+      </c>
+      <c r="H49" s="23">
+        <v>3.9187364944388201</v>
+      </c>
+      <c r="I49" s="23">
+        <v>1.8312892685683</v>
+      </c>
+      <c r="J49" s="2">
+        <v>5</v>
+      </c>
+      <c r="K49">
         <v>60</v>
       </c>
       <c r="Q49" s="28" t="s">
@@ -2053,7 +2053,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="47.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:27" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="28" t="s">
         <v>4</v>
       </c>
@@ -2066,25 +2066,25 @@
       <c r="D50" s="30">
         <v>1</v>
       </c>
-      <c r="E50" s="30">
-        <v>0.67</v>
-      </c>
-      <c r="F50" s="29">
-        <v>3.6</v>
-      </c>
-      <c r="G50" s="29">
-        <v>5.8</v>
-      </c>
-      <c r="H50" s="29">
-        <v>3.1</v>
-      </c>
-      <c r="I50" s="29">
-        <v>1.3</v>
-      </c>
-      <c r="J50" s="29">
-        <v>15</v>
-      </c>
-      <c r="K50" s="29">
+      <c r="E50" s="3">
+        <v>0.78395061728395099</v>
+      </c>
+      <c r="F50" s="23">
+        <v>3.7662814815966699</v>
+      </c>
+      <c r="G50" s="23">
+        <v>4.8888570983064898</v>
+      </c>
+      <c r="H50" s="23">
+        <v>3.2957187729732502</v>
+      </c>
+      <c r="I50" s="23">
+        <v>1.6489958987211799</v>
+      </c>
+      <c r="J50" s="2">
+        <v>5</v>
+      </c>
+      <c r="K50">
         <v>65</v>
       </c>
       <c r="Q50" s="31" t="s">
@@ -2121,7 +2121,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="70.8" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:27" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="31" t="s">
         <v>11</v>
       </c>
@@ -2134,25 +2134,25 @@
       <c r="D51" s="33">
         <v>1</v>
       </c>
-      <c r="E51" s="33">
-        <v>0.71</v>
-      </c>
-      <c r="F51" s="32">
-        <v>3.3</v>
-      </c>
-      <c r="G51" s="32">
-        <v>5.2</v>
-      </c>
-      <c r="H51" s="32">
-        <v>2.9</v>
-      </c>
-      <c r="I51" s="32">
-        <v>1.3</v>
-      </c>
-      <c r="J51" s="32">
-        <v>5</v>
-      </c>
-      <c r="K51" s="32">
+      <c r="E51" s="3">
+        <v>0.80555555555555602</v>
+      </c>
+      <c r="F51" s="23">
+        <v>3.6042473989701298</v>
+      </c>
+      <c r="G51" s="23">
+        <v>4.2251748337440098</v>
+      </c>
+      <c r="H51" s="23">
+        <v>3.0511811971656901</v>
+      </c>
+      <c r="I51" s="23">
+        <v>1.55722525088334</v>
+      </c>
+      <c r="J51" s="2">
+        <v>5</v>
+      </c>
+      <c r="K51">
         <v>65</v>
       </c>
       <c r="Q51" s="28" t="s">
@@ -2189,7 +2189,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:27" ht="70.8" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:27" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="28" t="s">
         <v>8</v>
       </c>
@@ -2202,26 +2202,26 @@
       <c r="D52" s="30">
         <v>1</v>
       </c>
-      <c r="E52" s="30">
-        <v>0.72</v>
-      </c>
-      <c r="F52" s="29">
-        <v>3.2</v>
-      </c>
-      <c r="G52" s="29">
-        <v>4.7</v>
-      </c>
-      <c r="H52" s="29">
-        <v>2.8</v>
-      </c>
-      <c r="I52" s="29">
-        <v>1.3</v>
-      </c>
-      <c r="J52" s="29">
-        <v>5</v>
-      </c>
-      <c r="K52" s="29">
-        <v>65</v>
+      <c r="E52" s="3">
+        <v>0.81481481481481499</v>
+      </c>
+      <c r="F52" s="23">
+        <v>3.5189800132604701</v>
+      </c>
+      <c r="G52" s="23">
+        <v>3.8136691510956102</v>
+      </c>
+      <c r="H52" s="23">
+        <v>2.8499983421883202</v>
+      </c>
+      <c r="I52" s="23">
+        <v>1.5828147353200701</v>
+      </c>
+      <c r="J52" s="2">
+        <v>5</v>
+      </c>
+      <c r="K52">
+        <v>70</v>
       </c>
       <c r="Q52" s="31" t="s">
         <v>3</v>
@@ -2257,7 +2257,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="70.8" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:27" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="28" t="s">
         <v>10</v>
       </c>
@@ -2270,25 +2270,25 @@
       <c r="D53" s="30">
         <v>1</v>
       </c>
-      <c r="E53" s="30">
-        <v>0.74</v>
-      </c>
-      <c r="F53" s="29">
-        <v>3</v>
-      </c>
-      <c r="G53" s="29">
-        <v>5.2</v>
-      </c>
-      <c r="H53" s="29">
-        <v>2.7</v>
-      </c>
-      <c r="I53" s="29">
-        <v>1.3</v>
-      </c>
-      <c r="J53" s="29">
-        <v>5</v>
-      </c>
-      <c r="K53" s="29">
+      <c r="E53" s="3">
+        <v>0.82253086419753096</v>
+      </c>
+      <c r="F53" s="23">
+        <v>3.2274161884264401</v>
+      </c>
+      <c r="G53" s="23">
+        <v>3.8777858727358701</v>
+      </c>
+      <c r="H53" s="23">
+        <v>2.76065726625606</v>
+      </c>
+      <c r="I53" s="23">
+        <v>1.6268928954965201</v>
+      </c>
+      <c r="J53" s="2">
+        <v>5</v>
+      </c>
+      <c r="K53">
         <v>70</v>
       </c>
       <c r="Q53" s="28" t="s">
@@ -2325,7 +2325,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="70.8" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:27" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="Q54" s="31" t="s">
         <v>11</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="70.8" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:27" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="Q55" s="28" t="s">
         <v>8</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="70.8" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:27" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="Q56" s="31" t="s">
         <v>10</v>
       </c>

</xml_diff>